<commit_message>
added post privacy check test with ddt
</commit_message>
<xml_diff>
--- a/src/main/resources/Credentials.xlsx
+++ b/src/main/resources/Credentials.xlsx
@@ -19,31 +19,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>yofigi5953@dewareff.com</t>
-  </si>
-  <si>
-    <t>Topaz96</t>
-  </si>
-  <si>
-    <t>yegati8771@dewareff.com</t>
-  </si>
-  <si>
-    <t>Lior96</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>privacyType</t>
+  </si>
+  <si>
+    <t>Only me</t>
+  </si>
+  <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>post text</t>
+  </si>
+  <si>
+    <t>Hello  only me post</t>
+  </si>
+  <si>
+    <t>Hello  Public post</t>
+  </si>
+  <si>
+    <t>expected result</t>
+  </si>
+  <si>
+    <t>Shared with Only me</t>
+  </si>
+  <si>
+    <t>Shared with Public</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,6 +64,12 @@
       <sz val="9.8000000000000007"/>
       <color rgb="FFA9B7C6"/>
       <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFE8EAED"/>
+      <name val="Consolas"/>
       <family val="3"/>
     </font>
   </fonts>
@@ -78,11 +93,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -363,42 +379,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed test result write to xlsx file
</commit_message>
<xml_diff>
--- a/src/main/resources/Credentials.xlsx
+++ b/src/main/resources/Credentials.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,39 +19,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>privacyType</t>
   </si>
   <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>post text</t>
+  </si>
+  <si>
+    <t>Hello  Public post</t>
+  </si>
+  <si>
+    <t>expected result</t>
+  </si>
+  <si>
+    <t>Shared with Only me</t>
+  </si>
+  <si>
+    <t>Shared with Public</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Helo only me post</t>
+  </si>
+  <si>
     <t>Only me</t>
   </si>
   <si>
-    <t>Public</t>
-  </si>
-  <si>
-    <t>post text</t>
-  </si>
-  <si>
-    <t>Hello  only me post</t>
-  </si>
-  <si>
-    <t>Hello  Public post</t>
-  </si>
-  <si>
-    <t>expected result</t>
-  </si>
-  <si>
-    <t>Shared with Only me</t>
-  </si>
-  <si>
-    <t>Shared with Public</t>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -379,51 +386,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.6640625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.44140625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.6640625"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="16.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
+      <c r="D3" t="s" s="0">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final fix for xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/Credentials.xlsx
+++ b/src/main/resources/Credentials.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>privacyType</t>
   </si>
@@ -30,9 +30,6 @@
     <t>post text</t>
   </si>
   <si>
-    <t>Hello  Public post</t>
-  </si>
-  <si>
     <t>expected result</t>
   </si>
   <si>
@@ -45,13 +42,16 @@
     <t>Result</t>
   </si>
   <si>
-    <t>Helo only me post</t>
-  </si>
-  <si>
     <t>Only me</t>
   </si>
   <si>
-    <t>Pass</t>
+    <t>Kuku 1</t>
+  </si>
+  <si>
+    <t>Kuku 2</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -408,21 +408,21 @@
         <v>2</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>10</v>
@@ -433,10 +433,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>10</v>

</xml_diff>